<commit_message>
switch: fix maxburst size on spreadsheet calc
</commit_message>
<xml_diff>
--- a/switch/CBS.xlsx
+++ b/switch/CBS.xlsx
@@ -358,20 +358,20 @@
   </sheetPr>
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O33" activeCellId="0" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.26"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -380,8 +380,6 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
       <c r="J3" s="1" t="s">
         <v>2</v>
       </c>
@@ -491,7 +489,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="5" t="n">
@@ -516,7 +514,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="5" t="n">
@@ -541,15 +539,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
       <c r="E11" s="1"/>
       <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K11" s="6" t="n">
-        <f aca="false">($C$4*((K10-K9)/(-K8)))/8</f>
-        <v>0.0132689268926893</v>
+        <f aca="false">$C$4*((K10-K9)/(-K8))</f>
+        <v>0.106151415141514</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>8</v>
@@ -571,9 +567,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -582,8 +576,6 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
       <c r="J14" s="1" t="s">
         <v>2</v>
       </c>
@@ -595,8 +587,6 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
       <c r="J15" s="1" t="s">
         <v>5</v>
       </c>
@@ -609,7 +599,6 @@
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="0"/>
       <c r="J16" s="1" t="s">
         <v>7</v>
       </c>
@@ -625,13 +614,12 @@
       <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="0"/>
       <c r="J17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K17" s="6" t="n">
         <f aca="false">K6+K11</f>
-        <v>1.52726892689269</v>
+        <v>1.62015141514151</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>8</v>
@@ -644,7 +632,6 @@
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="0"/>
       <c r="J18" s="1" t="s">
         <v>12</v>
       </c>
@@ -660,7 +647,6 @@
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="0"/>
       <c r="J19" s="1" t="s">
         <v>15</v>
       </c>
@@ -676,7 +662,6 @@
       <c r="B20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="0"/>
       <c r="J20" s="1" t="s">
         <v>18</v>
       </c>
@@ -685,58 +670,51 @@
         <v>-1.3626</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="0"/>
       <c r="J21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K21" s="6" t="n">
         <f aca="false">K17*(K18/$C$4)</f>
-        <v>0.152726892689269</v>
+        <v>0.162015141514151</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="0"/>
       <c r="J22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="6" t="n">
-        <f aca="false">($C$4*((K21-K20)/(-K19)))/8</f>
-        <v>0.210462068429065</v>
+        <f aca="false">$C$4*((K21-K20)/(-K19))</f>
+        <v>1.69401682390461</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="0"/>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="M24" s="0" t="s">
+      <c r="M24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="N24" s="2" t="s">
@@ -748,7 +726,6 @@
       <c r="B25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="0"/>
       <c r="J25" s="1" t="s">
         <v>2</v>
       </c>
@@ -762,15 +739,13 @@
         <v>2</v>
       </c>
       <c r="O25" s="3" t="n">
-        <v>1000000</v>
+        <v>300000</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
       <c r="J26" s="1" t="s">
         <v>5</v>
       </c>
@@ -783,12 +758,10 @@
       </c>
       <c r="O26" s="4" t="n">
         <f aca="false">O25/$C$4</f>
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
       <c r="J27" s="1" t="s">
         <v>7</v>
       </c>
@@ -811,14 +784,12 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
       <c r="J28" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K28" s="6" t="n">
         <f aca="false">K17+K22</f>
-        <v>1.73773099532175</v>
+        <v>3.31416823904613</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>8</v>
@@ -828,7 +799,7 @@
       </c>
       <c r="O28" s="6" t="n">
         <f aca="false">K28+K33</f>
-        <v>1.98128508892556</v>
+        <v>5.65671029880766</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>8</v>
@@ -856,18 +827,18 @@
       </c>
       <c r="O29" s="7" t="n">
         <f aca="false">$C$4*O26</f>
-        <v>1000000</v>
+        <v>300000</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>1</v>
+        <v>6000</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>15</v>
@@ -884,15 +855,13 @@
       </c>
       <c r="O30" s="7" t="n">
         <f aca="false">O29-$C$4</f>
-        <v>0</v>
+        <v>-700000</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
       <c r="J31" s="1" t="s">
         <v>18</v>
       </c>
@@ -901,51 +870,48 @@
         <v>-1.2112</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="O31" s="6" t="n">
         <f aca="false">O27*(O30/$C$4)</f>
-        <v>0</v>
+        <v>-1.0598</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
       <c r="J32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K32" s="6" t="n">
         <f aca="false">K28*(K29/$C$4)</f>
-        <v>0.347546199064351</v>
+        <v>0.662833647809225</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="O32" s="6" t="n">
         <f aca="false">O28*(O29/$C$4)</f>
-        <v>1.98128508892556</v>
+        <v>1.6970130896423</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0"/>
       <c r="J33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="6" t="n">
-        <f aca="false">($C$4*((K32-K31)/(-K30)))/8</f>
-        <v>0.243554093603805</v>
+        <f aca="false">$C$4*((K32-K31)/(-K30))</f>
+        <v>2.34254205976153</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>8</v>
@@ -953,9 +919,9 @@
       <c r="N33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O33" s="6" t="e">
-        <f aca="false">($C$4*((O32-O31)/(-O30)))/8</f>
-        <v>#DIV/0!</v>
+      <c r="O33" s="6" t="n">
+        <f aca="false">$C$4*((O32-O31)/(-O30))</f>
+        <v>3.93830441377471</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>8</v>
@@ -963,34 +929,34 @@
     </row>
     <row r="34" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="8" t="str">
-        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":1 handle 11 cbs \
+        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":1 handle 6001 cbs \
         idleslope ",K7," sendslope ",K8," hicredit ",_xlfn.CEILING.MATH(K10*1000)," locredit ",_xlfn.CEILING.MATH(K9*1000))</f>
-        <v>sudo tc qdisc replace dev enp4s0f1 parent 1:1 handle 11 cbs \
+        <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:1 handle 6001 cbs \
         idleslope 100 sendslope -999900 hicredit 1 locredit -105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="8" t="str">
-        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":2 handle 12 cbs \
+        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":2 handle 6002 cbs \
         idleslope ",K18," sendslope ",K19," hicredit ",_xlfn.CEILING.MATH(K21*1000)," locredit ",_xlfn.CEILING.MATH(K20*1000))</f>
-        <v>sudo tc qdisc replace dev enp4s0f1 parent 1:2 handle 12 cbs \
-        idleslope 100000 sendslope -900000 hicredit 153 locredit -1362</v>
+        <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:2 handle 6002 cbs \
+        idleslope 100000 sendslope -900000 hicredit 163 locredit -1362</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="8" t="str">
-        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":3 handle 13 cbs \
+        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":3 handle 6003 cbs \
         idleslope ",K29," sendslope ",K30," hicredit ",_xlfn.CEILING.MATH(K32*1000)," locredit ",_xlfn.CEILING.MATH(K31*1000))</f>
-        <v>sudo tc qdisc replace dev enp4s0f1 parent 1:3 handle 13 cbs \
-        idleslope 200000 sendslope -800000 hicredit 348 locredit -1211</v>
+        <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:3 handle 6003 cbs \
+        idleslope 200000 sendslope -800000 hicredit 663 locredit -1211</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="8" t="str">
-        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":4 handle 14 cbs \
+        <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":4 handle 6004 cbs \
         idleslope ",O29," sendslope ",O30," hicredit ",_xlfn.CEILING.MATH(O32*1000)," locredit ",_xlfn.CEILING.MATH(O31*1000))</f>
-        <v>sudo tc qdisc replace dev enp4s0f1 parent 1:4 handle 14 cbs \
-        idleslope 1000000 sendslope 0 hicredit 1982 locredit 0</v>
+        <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:4 handle 6004 cbs \
+        idleslope 300000 sendslope -700000 hicredit 1698 locredit -1059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switch: Add TAS spreadsheet
also update CBS
</commit_message>
<xml_diff>
--- a/switch/CBS.xlsx
+++ b/switch/CBS.xlsx
@@ -158,11 +158,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -275,7 +276,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -358,8 +359,8 @@
   </sheetPr>
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O33" activeCellId="0" sqref="O33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +385,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>100</v>
+        <v>600000</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>3</v>
@@ -405,7 +406,7 @@
       </c>
       <c r="K4" s="4" t="n">
         <f aca="false">K3/$C$4</f>
-        <v>0.0001</v>
+        <v>0.6</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>6</v>
@@ -416,8 +417,8 @@
         <v>7</v>
       </c>
       <c r="K5" s="5" t="n">
-        <f aca="false">C7</f>
-        <v>0.106</v>
+        <f aca="false">1542/1000</f>
+        <v>1.542</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>8</v>
@@ -429,7 +430,7 @@
       </c>
       <c r="K6" s="6" t="n">
         <f aca="false">C12</f>
-        <v>1.514</v>
+        <v>1.542</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>8</v>
@@ -454,7 +455,7 @@
       </c>
       <c r="K7" s="7" t="n">
         <f aca="false">C4*K4</f>
-        <v>100</v>
+        <v>600000</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>3</v>
@@ -479,7 +480,7 @@
       </c>
       <c r="K8" s="7" t="n">
         <f aca="false">K7-C4</f>
-        <v>-999900</v>
+        <v>-400000</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>3</v>
@@ -504,7 +505,7 @@
       </c>
       <c r="K9" s="6" t="n">
         <f aca="false">K5*(K8/C4)</f>
-        <v>-0.1059894</v>
+        <v>-0.6168</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>8</v>
@@ -518,8 +519,8 @@
         <v>20</v>
       </c>
       <c r="C10" s="5" t="n">
-        <f aca="false">1514/1000</f>
-        <v>1.514</v>
+        <f aca="false">1542/1000</f>
+        <v>1.542</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -529,7 +530,7 @@
       </c>
       <c r="K10" s="6" t="n">
         <f aca="false">K6*(K7/$C$4)</f>
-        <v>0.0001514</v>
+        <v>0.9252</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>8</v>
@@ -545,7 +546,7 @@
       </c>
       <c r="K11" s="6" t="n">
         <f aca="false">$C$4*((K10-K9)/(-K8))</f>
-        <v>0.106151415141514</v>
+        <v>3.855</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>8</v>
@@ -560,7 +561,7 @@
       </c>
       <c r="C12" s="5" t="n">
         <f aca="false">MAX(C7:C10)</f>
-        <v>1.514</v>
+        <v>1.542</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -580,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>3</v>
@@ -592,7 +593,7 @@
       </c>
       <c r="K15" s="4" t="n">
         <f aca="false">K14/$C$4</f>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,8 +604,8 @@
         <v>7</v>
       </c>
       <c r="K16" s="5" t="n">
-        <f aca="false">C8</f>
-        <v>1.514</v>
+        <f aca="false">1542/1000</f>
+        <v>1.542</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>8</v>
@@ -619,7 +620,7 @@
       </c>
       <c r="K17" s="6" t="n">
         <f aca="false">K6+K11</f>
-        <v>1.62015141514151</v>
+        <v>5.397</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>8</v>
@@ -637,7 +638,7 @@
       </c>
       <c r="K18" s="7" t="n">
         <f aca="false">$C$4*K15</f>
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>3</v>
@@ -652,7 +653,7 @@
       </c>
       <c r="K19" s="7" t="n">
         <f aca="false">K18-$C$4</f>
-        <v>-900000</v>
+        <v>-500000</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>3</v>
@@ -667,7 +668,7 @@
       </c>
       <c r="K20" s="6" t="n">
         <f aca="false">K16*(K19/$C$4)</f>
-        <v>-1.3626</v>
+        <v>-0.771</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>8</v>
@@ -682,7 +683,7 @@
       </c>
       <c r="K21" s="6" t="n">
         <f aca="false">K17*(K18/$C$4)</f>
-        <v>0.162015141514151</v>
+        <v>2.6985</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>8</v>
@@ -697,7 +698,7 @@
       </c>
       <c r="K22" s="6" t="n">
         <f aca="false">$C$4*((K21-K20)/(-K19))</f>
-        <v>1.69401682390461</v>
+        <v>6.939</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>8</v>
@@ -730,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="3" t="n">
-        <v>200000</v>
+        <v>999999</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>3</v>
@@ -739,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="O25" s="3" t="n">
-        <v>300000</v>
+        <v>1000000</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>3</v>
@@ -751,14 +752,14 @@
       </c>
       <c r="K26" s="4" t="n">
         <f aca="false">K25/$C$4</f>
-        <v>0.2</v>
+        <v>0.999999</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O26" s="4" t="n">
         <f aca="false">O25/$C$4</f>
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,7 +778,7 @@
       </c>
       <c r="O27" s="5" t="n">
         <f aca="false">C10</f>
-        <v>1.514</v>
+        <v>1.542</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>8</v>
@@ -789,7 +790,7 @@
       </c>
       <c r="K28" s="6" t="n">
         <f aca="false">K17+K22</f>
-        <v>3.31416823904613</v>
+        <v>12.336</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>8</v>
@@ -799,7 +800,7 @@
       </c>
       <c r="O28" s="6" t="n">
         <f aca="false">K28+K33</f>
-        <v>5.65671029880766</v>
+        <v>12336001.514</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>8</v>
@@ -817,7 +818,7 @@
       </c>
       <c r="K29" s="7" t="n">
         <f aca="false">$C$4*K26</f>
-        <v>200000</v>
+        <v>999999</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>3</v>
@@ -827,7 +828,7 @@
       </c>
       <c r="O29" s="7" t="n">
         <f aca="false">$C$4*O26</f>
-        <v>300000</v>
+        <v>1000000</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>3</v>
@@ -845,7 +846,7 @@
       </c>
       <c r="K30" s="7" t="n">
         <f aca="false">K29-$C$4</f>
-        <v>-800000</v>
+        <v>-1</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>3</v>
@@ -855,7 +856,7 @@
       </c>
       <c r="O30" s="7" t="n">
         <f aca="false">O29-$C$4</f>
-        <v>-700000</v>
+        <v>0</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>3</v>
@@ -867,7 +868,7 @@
       </c>
       <c r="K31" s="6" t="n">
         <f aca="false">K27*(K30/$C$4)</f>
-        <v>-1.2112</v>
+        <v>-1.514E-006</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>8</v>
@@ -877,7 +878,7 @@
       </c>
       <c r="O31" s="6" t="n">
         <f aca="false">O27*(O30/$C$4)</f>
-        <v>-1.0598</v>
+        <v>0</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>8</v>
@@ -889,7 +890,7 @@
       </c>
       <c r="K32" s="6" t="n">
         <f aca="false">K28*(K29/$C$4)</f>
-        <v>0.662833647809225</v>
+        <v>12.335987664</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>8</v>
@@ -899,7 +900,7 @@
       </c>
       <c r="O32" s="6" t="n">
         <f aca="false">O28*(O29/$C$4)</f>
-        <v>1.6970130896423</v>
+        <v>12336001.514</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>8</v>
@@ -911,7 +912,7 @@
       </c>
       <c r="K33" s="6" t="n">
         <f aca="false">$C$4*((K32-K31)/(-K30))</f>
-        <v>2.34254205976153</v>
+        <v>12335989.178</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>8</v>
@@ -919,9 +920,9 @@
       <c r="N33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O33" s="6" t="n">
+      <c r="O33" s="6" t="e">
         <f aca="false">$C$4*((O32-O31)/(-O30))</f>
-        <v>3.93830441377471</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>8</v>
@@ -932,7 +933,7 @@
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":1 handle 6001 cbs \
         idleslope ",K7," sendslope ",K8," hicredit ",_xlfn.CEILING.MATH(K10*1000)," locredit ",_xlfn.CEILING.MATH(K9*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:1 handle 6001 cbs \
-        idleslope 100 sendslope -999900 hicredit 1 locredit -105</v>
+        idleslope 600000 sendslope -400000 hicredit 926 locredit -616</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,7 +941,7 @@
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":2 handle 6002 cbs \
         idleslope ",K18," sendslope ",K19," hicredit ",_xlfn.CEILING.MATH(K21*1000)," locredit ",_xlfn.CEILING.MATH(K20*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:2 handle 6002 cbs \
-        idleslope 100000 sendslope -900000 hicredit 163 locredit -1362</v>
+        idleslope 500000 sendslope -500000 hicredit 2699 locredit -771</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,15 +949,15 @@
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":3 handle 6003 cbs \
         idleslope ",K29," sendslope ",K30," hicredit ",_xlfn.CEILING.MATH(K32*1000)," locredit ",_xlfn.CEILING.MATH(K31*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:3 handle 6003 cbs \
-        idleslope 200000 sendslope -800000 hicredit 663 locredit -1211</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        idleslope 999999 sendslope -1 hicredit 12336 locredit 0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="8" t="str">
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":4 handle 6004 cbs \
         idleslope ",O29," sendslope ",O30," hicredit ",_xlfn.CEILING.MATH(O32*1000)," locredit ",_xlfn.CEILING.MATH(O31*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:4 handle 6004 cbs \
-        idleslope 300000 sendslope -700000 hicredit 1698 locredit -1059</v>
+        idleslope 1000000 sendslope 0 hicredit 12336001514 locredit 0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests: rename tests script folders
</commit_message>
<xml_diff>
--- a/switch/CBS.xlsx
+++ b/switch/CBS.xlsx
@@ -277,7 +277,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -359,8 +359,8 @@
   </sheetPr>
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,7 +385,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>3</v>
@@ -406,7 +406,7 @@
       </c>
       <c r="K4" s="4" t="n">
         <f aca="false">K3/$C$4</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>6</v>
@@ -455,7 +455,7 @@
       </c>
       <c r="K7" s="7" t="n">
         <f aca="false">C4*K4</f>
-        <v>600000</v>
+        <v>400000</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>3</v>
@@ -480,7 +480,7 @@
       </c>
       <c r="K8" s="7" t="n">
         <f aca="false">K7-C4</f>
-        <v>-400000</v>
+        <v>-600000</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>3</v>
@@ -505,7 +505,7 @@
       </c>
       <c r="K9" s="6" t="n">
         <f aca="false">K5*(K8/C4)</f>
-        <v>-0.6168</v>
+        <v>-0.9252</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>8</v>
@@ -530,7 +530,7 @@
       </c>
       <c r="K10" s="6" t="n">
         <f aca="false">K6*(K7/$C$4)</f>
-        <v>0.9252</v>
+        <v>0.6168</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>8</v>
@@ -546,7 +546,7 @@
       </c>
       <c r="K11" s="6" t="n">
         <f aca="false">$C$4*((K10-K9)/(-K8))</f>
-        <v>3.855</v>
+        <v>2.57</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>8</v>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>500000</v>
+        <v>300000</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>3</v>
@@ -593,7 +593,7 @@
       </c>
       <c r="K15" s="4" t="n">
         <f aca="false">K14/$C$4</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,7 +620,7 @@
       </c>
       <c r="K17" s="6" t="n">
         <f aca="false">K6+K11</f>
-        <v>5.397</v>
+        <v>4.112</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>8</v>
@@ -638,7 +638,7 @@
       </c>
       <c r="K18" s="7" t="n">
         <f aca="false">$C$4*K15</f>
-        <v>500000</v>
+        <v>300000</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>3</v>
@@ -653,7 +653,7 @@
       </c>
       <c r="K19" s="7" t="n">
         <f aca="false">K18-$C$4</f>
-        <v>-500000</v>
+        <v>-700000</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>3</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="K20" s="6" t="n">
         <f aca="false">K16*(K19/$C$4)</f>
-        <v>-0.771</v>
+        <v>-1.0794</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>8</v>
@@ -683,7 +683,7 @@
       </c>
       <c r="K21" s="6" t="n">
         <f aca="false">K17*(K18/$C$4)</f>
-        <v>2.6985</v>
+        <v>1.2336</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>8</v>
@@ -698,7 +698,7 @@
       </c>
       <c r="K22" s="6" t="n">
         <f aca="false">$C$4*((K21-K20)/(-K19))</f>
-        <v>6.939</v>
+        <v>3.30428571428571</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>8</v>
@@ -790,7 +790,7 @@
       </c>
       <c r="K28" s="6" t="n">
         <f aca="false">K17+K22</f>
-        <v>12.336</v>
+        <v>7.41628571428571</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>8</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="O28" s="6" t="n">
         <f aca="false">K28+K33</f>
-        <v>12336001.514</v>
+        <v>7416287.22828571</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>8</v>
@@ -890,7 +890,7 @@
       </c>
       <c r="K32" s="6" t="n">
         <f aca="false">K28*(K29/$C$4)</f>
-        <v>12.335987664</v>
+        <v>7.416278298</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>8</v>
@@ -900,7 +900,7 @@
       </c>
       <c r="O32" s="6" t="n">
         <f aca="false">O28*(O29/$C$4)</f>
-        <v>12336001.514</v>
+        <v>7416287.22828571</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>8</v>
@@ -912,7 +912,7 @@
       </c>
       <c r="K33" s="6" t="n">
         <f aca="false">$C$4*((K32-K31)/(-K30))</f>
-        <v>12335989.178</v>
+        <v>7416279.812</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>8</v>
@@ -933,7 +933,7 @@
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":1 handle 6001 cbs \
         idleslope ",K7," sendslope ",K8," hicredit ",_xlfn.CEILING.MATH(K10*1000)," locredit ",_xlfn.CEILING.MATH(K9*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:1 handle 6001 cbs \
-        idleslope 600000 sendslope -400000 hicredit 926 locredit -616</v>
+        idleslope 400000 sendslope -600000 hicredit 617 locredit -925</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,7 +941,7 @@
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":2 handle 6002 cbs \
         idleslope ",K18," sendslope ",K19," hicredit ",_xlfn.CEILING.MATH(K21*1000)," locredit ",_xlfn.CEILING.MATH(K20*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:2 handle 6002 cbs \
-        idleslope 500000 sendslope -500000 hicredit 2699 locredit -771</v>
+        idleslope 300000 sendslope -700000 hicredit 1234 locredit -1079</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,15 +949,15 @@
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":3 handle 6003 cbs \
         idleslope ",K29," sendslope ",K30," hicredit ",_xlfn.CEILING.MATH(K32*1000)," locredit ",_xlfn.CEILING.MATH(K31*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:3 handle 6003 cbs \
-        idleslope 999999 sendslope -1 hicredit 12336 locredit 0</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        idleslope 999999 sendslope -1 hicredit 7417 locredit 0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="8" t="str">
         <f aca="false">_xlfn.CONCAT("sudo tc qdisc replace dev ",$C$29," parent ",$C$30,":4 handle 6004 cbs \
         idleslope ",O29," sendslope ",O30," hicredit ",_xlfn.CEILING.MATH(O32*1000)," locredit ",_xlfn.CEILING.MATH(O31*1000))</f>
         <v>sudo tc qdisc replace dev enp4s0f1 parent 6000:4 handle 6004 cbs \
-        idleslope 1000000 sendslope 0 hicredit 12336001514 locredit 0</v>
+        idleslope 1000000 sendslope 0 hicredit 7416287229 locredit 0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>